<commit_message>
two bugs left for fixing
</commit_message>
<xml_diff>
--- a/prepareExcel/Titelblatt.xlsx
+++ b/prepareExcel/Titelblatt.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\szh.loc\ssz\data\Projekte\Mietpreisstrukturerhebung\99_Shiny_App\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\szh.loc\ssz\data\Projekte\Mietpreisstrukturerhebung\99_Shiny_App\prepareExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Napfgasse 6, 8022 Zürich</t>
   </si>
@@ -64,57 +64,60 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Preis in CHF pro Quadratmeter bebautem Land</t>
-  </si>
-  <si>
-    <t>Anzahl Handänderungen</t>
-  </si>
-  <si>
-    <t>Anonymisierung Anzahl Handänderungen</t>
-  </si>
-  <si>
-    <t>In Kategorien mit weniger als vier Handänderungen wird aus Datenschutzgründen anstelle der genauen Anzahl Handänderungen der Wert «1–3» angezeigt.</t>
-  </si>
-  <si>
-    <t>Umgesetzte Fläche (m2)</t>
-  </si>
-  <si>
-    <t>Transaktionsvolumen (CHF)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vergleich mit früher publizierten Tabellen: </t>
-  </si>
-  <si>
-    <t>Da im vergangenen Jahr diverse Datenbereinigungen vorgenommen worden sind, können die hier publizierten Werte aufgrund besserer Datenqualität von früher publizierten Werten abweichen.</t>
-  </si>
-  <si>
-    <t>Median-Quadratmeterpreise von allen im Freihandkauf in der Stadt Zürich gehandelten Grundstücken, gruppiert nach Hauptbebauungsart und Handänderungsjahr. Es wurden nur Handänderungen von Grundstücken in Bauzonen (ohne Industriezonen und ohne Zonen für öffentliche Bauten) berücksichtigt.
-Zwei Tabellentabs, jeweils mit und ohne anteilsmässiger Berücksichtigung von Transaktionen im Stockwerkeigentum</t>
-  </si>
-  <si>
-    <t>Anzahl Freihandkäufe in der Stadt Zürich, gruppiert nach Hauptbebauungsart und Handänderungsjahr. Es wurden nur Handänderungen von Grundstücken in Bauzonen (ohne Industriezonen und ohne Zonen für öffentliche Bauten) berücksichtigt.
-Zwei Tabellentabs, jeweils mit und ohne Berücksichtigung von Transaktionen im Stockwerkeigentum</t>
-  </si>
-  <si>
-    <t>Im Freihandkauf umgesetzte Fläche in der Stadt Zürich, gruppiert nach Hauptbebauungsart und Handänderungsjahr. Es wurden nur Handänderungen von Grundstücken in Bauzonen (ohne Industriezonen und ohne Zonen für öffentliche Bauten) berücksichtigt.
-Zwei Tabellentabs, jeweils mit und ohne anteilsmässiger Berücksichtigung von Transaktionen im Stockwerkeigentum</t>
-  </si>
-  <si>
-    <t>Im Freihandkauf umgesetztes Handelsvolumen von Grundstücken in der Stadt Zürich, gruppiert nach Hauptbebauungsart und Handänderungsjahr. Es wurden nur Handänderungen von Grundstücken in Bauzonen (ohne Industriezonen und ohne Zonen für öffentliche Bauten) berücksichtigt.
-Zwei Tabellentabs, jeweils mit und ohne anteilsmässiger Berücksichtigung von Transaktionen im Stockwerkeigentum</t>
-  </si>
-  <si>
     <t>Begriff</t>
   </si>
   <si>
     <t>Definition</t>
+  </si>
+  <si>
+    <t>Mietpreiserhebung (MPE)</t>
+  </si>
+  <si>
+    <t>Die Mietpreiserhebung (MPE) gibt die geschätzten Mietpreise in der Stadt Zürich per Stichmonat April 2022 wieder. Die Erhebung ist als Zweischichtenmodell konzipiert und basiert auf automatisierten Datenlieferungen von Verwaltungen (Schicht 1) und einer ergänzenden Zufallsstichprobe (Schicht 2). Die Resultate beziehen sich ausschliesslich auf die Grössenklassen der 2-, 3- und 4-Zimmer-Wohnungen, die über 80 Prozent des Mietwohnungsbestandes abdecken. Vgl. auch den publizierten Methodikbericht.</t>
+  </si>
+  <si>
+    <t>Gemeinnützigkeit</t>
+  </si>
+  <si>
+    <t>Zu den gemeinnützigen gehören zunächst alle Wohnungen, die im Besitz der Stadt oder von Genossenschaften, Vereinen oder Stiftungen sind und nach dem Grundsatz der Kostenmiete bewirtschaftet werden. Ferner gehören auch Wohnungen dazu, deren Eigentümerschaft als gemeinnützig im weiteren Sinne gilt und ihre Mietobjekte nicht ausschliesslich nach dem Prinzip der Kostenmiete vermietet (bestimmte Stiftungen, Vereine und Aktiengesellschaften). Mit der Kostenmiete werden die Schuldzinsen und die Verwaltungskosten beglichen, der Unterhalt und Werterhalt der Liegenschaften sowie die Rückstellungen zur Erneuerung sichergestellt. Mittel- bis langfristig bewirkt die Kostenmiete deutlich günstigere Mieten als bei vergleichbaren Objekten auf dem Wohnungsmarkt.</t>
+  </si>
+  <si>
+    <t>Raumeinheit Stadtquartiere</t>
+  </si>
+  <si>
+    <t>Für eine Stichprobenerhebung wie die MPE sind die Stadtquartiere zum Teil klein. Auf Stufe Stadtquartier ist deshalb keine Differenzierung der Mietpreise nach Gemeinnützigkeit möglich. Die Mietpreise können nur für den Gesamtwohnungsbestand ausgewiesen werden.</t>
+  </si>
+  <si>
+    <t>Raumeinheit Quartiergruppen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Da auf Stufe Stadtquartier keine Differenzierung der Mietpreise nach Gemeinnützigkeit möglich ist, in grösseren Quartieren hingegen schon, werden kleinere oder einseitig strukturierte Quartiere  deshalb zu Quartiergruppen zusammengefasst. Dazu wurden die Quartiere der Kreise 1, 2, 5 und 8 zusammengelegt. Ferner werden zehn weitere Quartiere zu Paaren vereinigt Fluntern und Hottingen, Hirslanden und Witikon, Alt-Wiedikon und Friesenberg, Werd und Langstrasse sowie Saatlen und Schwamendingen-Mitte. 
+</t>
+  </si>
+  <si>
+    <t>Median (Zentralwert)</t>
+  </si>
+  <si>
+    <t>Der Median ist der Wert, der genau in der Mitte einer Datenreihe liegt, die nach der Größe geordnet ist. Aufgrund dieser zentralen Lage wird er auch Zentralwert genannt. Der Median halbiert die Datenreihe, sodass eine Hälfte der Daten unterhalb und die andere Hälfte oberhalb des Medians in der geordneten Reihe liegt.</t>
+  </si>
+  <si>
+    <t>Konfidenzintervall</t>
+  </si>
+  <si>
+    <t>Die geschätzten Preise sind mit 95-%-Konfidenzintervallen unterlegt. Diese bezeichnen den Bereich, der bei unendlicher Wiederholung eines Zufallsexperiments mit einer Wahrscheinlichkeit von 95 Prozent den wahren Wert der Grundgesamtheit einschliesst. In der MPE liegen die 95-%-Konfidenzintervalle gesamtstädtisch ungefähr bei +/-2 Prozent der ausgewiesenen Medianpreise und Mittelwerte. Bei kleineren Raumeinheiten (z.B. Quartiere) sind die Unsicherheiten höher; die Konfidenzintervalle der ausgewiesenen Werte liegen im Bereich von 4 bis 8 Prozent und können unter Umständen bis gegen 20 Prozent steigen.</t>
+  </si>
+  <si>
+    <t>Abfragetool MPE</t>
+  </si>
+  <si>
+    <t>Die Detaildaten der Mietpreiserhebung 2022 sind auf einem Abruftool verfügbar, das erreichbar ist unter: https://www.stadt-zuerich.ch/prd/de/index/statistik/themen/bauen-wohnen/mietpreise.html</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,17 +128,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -147,6 +139,36 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -168,34 +190,45 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="Standard 2" xfId="1"/>
+    <cellStyle name="Standard 2 2" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -514,73 +547,79 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.1" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="70.625" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="11" style="3"/>
+    <col min="1" max="1" width="27.625" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="70.625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="16384" width="11" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="5" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:2" s="3" customFormat="1" ht="14.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" s="5" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B7" s="7" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="54.95" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>21</v>
+    <row r="8" spans="1:2" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>